<commit_message>
Re-run all analyses dated today. Run regression analysis with traits as outcomes.
</commit_message>
<xml_diff>
--- a/data/for_plotting/betas.xlsx
+++ b/data/for_plotting/betas.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="20">
   <si>
     <t>Outcome</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>no_effort</t>
+  </si>
+  <si>
+    <t>cfr_species</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -512,7 +515,7 @@
         <v>0.093618355691432953</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>17</v>
@@ -529,28 +532,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
-        <v>0.38143458962440491</v>
+        <v>0.3501109778881073</v>
       </c>
       <c r="E3" s="2">
-        <v>0.078820571303367615</v>
+        <v>0.091486096382141113</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="2">
-        <v>0.22379344701766968</v>
+        <v>0.16713878512382507</v>
       </c>
       <c r="I3" s="2">
-        <v>0.53907573223114014</v>
+        <v>0.53308320045471191</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
@@ -558,161 +561,161 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
-        <v>0.1902749091386795</v>
+        <v>0.37285584211349487</v>
       </c>
       <c r="E4" s="2">
-        <v>0.029175437986850739</v>
+        <v>0.085471294820308685</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="2">
-        <v>0.13192403316497803</v>
+        <v>0.2019132524728775</v>
       </c>
       <c r="I4" s="2">
-        <v>0.24862578511238098</v>
+        <v>0.54379844665527344</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>0.39644512534141541</v>
+        <v>0.89913344383239746</v>
       </c>
       <c r="E5" s="2">
-        <v>0.07859821617603302</v>
+        <v>0.020791295915842056</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="2">
-        <v>0.23924869298934937</v>
+        <v>0.85755085945129395</v>
       </c>
       <c r="I5" s="2">
-        <v>0.55364155769348145</v>
+        <v>0.94071602821350098</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <v>0.19427020847797394</v>
+        <v>0.89727693796157837</v>
       </c>
       <c r="E6" s="2">
-        <v>0.027645748108625412</v>
+        <v>0.01982947438955307</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="2">
-        <v>0.13897871971130371</v>
+        <v>0.85761797428131104</v>
       </c>
       <c r="I6" s="2">
-        <v>0.24956169724464417</v>
+        <v>0.9369359016418457</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2">
-        <v>0.4135589599609375</v>
+        <v>0.89582264423370361</v>
       </c>
       <c r="E7" s="2">
-        <v>0.072071172297000885</v>
+        <v>0.019301192834973335</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="2">
-        <v>0.26941663026809692</v>
+        <v>0.85722023248672485</v>
       </c>
       <c r="I7" s="2">
-        <v>0.55770128965377808</v>
+        <v>0.93442505598068237</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2">
-        <v>0.18998445570468903</v>
+        <v>0.2708798348903656</v>
       </c>
       <c r="E8" s="2">
-        <v>0.0245700404047966</v>
+        <v>0.039570342749357224</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="2">
-        <v>0.14084437489509583</v>
+        <v>0.19173914194107056</v>
       </c>
       <c r="I8" s="2">
-        <v>0.23912453651428223</v>
+        <v>0.35002052783966064</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2">
-        <v>0.89913344383239746</v>
+        <v>0.27627730369567871</v>
       </c>
       <c r="E9" s="2">
-        <v>0.020791295915842056</v>
+        <v>0.036794524639844894</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -721,27 +724,27 @@
         <v>17</v>
       </c>
       <c r="H9" s="2">
-        <v>0.85755085945129395</v>
+        <v>0.20268824696540833</v>
       </c>
       <c r="I9" s="2">
-        <v>0.94071602821350098</v>
+        <v>0.3498663604259491</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
-        <v>0.89680230617523193</v>
+        <v>0.28031918406486511</v>
       </c>
       <c r="E10" s="2">
-        <v>0.016864331439137459</v>
+        <v>0.038133770227432251</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -750,10 +753,10 @@
         <v>17</v>
       </c>
       <c r="H10" s="2">
-        <v>0.86307364702224731</v>
+        <v>0.20405164361000061</v>
       </c>
       <c r="I10" s="2">
-        <v>0.93053096532821655</v>
+        <v>0.35658672451972961</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
@@ -761,28 +764,28 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2">
-        <v>0.0016589714214205742</v>
+        <v>0.29589375853538513</v>
       </c>
       <c r="E11" s="2">
-        <v>0.0049769198521971703</v>
+        <v>0.081302262842655182</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" s="2">
-        <v>-0.0082948682829737663</v>
+        <v>0.13328923285007477</v>
       </c>
       <c r="I11" s="2">
-        <v>0.011612811125814915</v>
+        <v>0.45849829912185669</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.2">
@@ -790,28 +793,28 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="2">
-        <v>0.89658713340759277</v>
+        <v>0.30266293883323669</v>
       </c>
       <c r="E12" s="2">
-        <v>0.015825795009732246</v>
+        <v>0.078538224101066589</v>
       </c>
       <c r="F12" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="2">
-        <v>0.86493551731109619</v>
+        <v>0.14558649063110352</v>
       </c>
       <c r="I12" s="2">
-        <v>0.92823874950408936</v>
+        <v>0.45973938703536987</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.2">
@@ -819,86 +822,86 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
-        <v>0.00049429910723119974</v>
+        <v>0.32400384545326233</v>
       </c>
       <c r="E13" s="2">
-        <v>0.0047461548820137978</v>
+        <v>0.071458756923675537</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H13" s="2">
-        <v>-0.0089980103075504303</v>
+        <v>0.18108633160591125</v>
       </c>
       <c r="I13" s="2">
-        <v>0.0099866092205047607</v>
+        <v>0.4669213593006134</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2">
-        <v>0.89520347118377686</v>
+        <v>0.063580483198165894</v>
       </c>
       <c r="E14" s="2">
-        <v>0.01529624592512846</v>
+        <v>0.035771388560533524</v>
       </c>
       <c r="F14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" s="2">
-        <v>0.86461097002029419</v>
+        <v>-0.0079622939229011536</v>
       </c>
       <c r="I14" s="2">
-        <v>0.92579597234725952</v>
+        <v>0.13512325286865234</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2">
-        <v>0.00044509768486022949</v>
+        <v>0.053387299180030823</v>
       </c>
       <c r="E15" s="2">
-        <v>0.0047815782018005848</v>
+        <v>0.035245683044195175</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H15" s="2">
-        <v>-0.0091180587187409401</v>
+        <v>-0.017104066908359528</v>
       </c>
       <c r="I15" s="2">
-        <v>0.010008254088461399</v>
+        <v>0.12387866526842117</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.2">
@@ -906,28 +909,28 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2">
-        <v>0.2708798348903656</v>
+        <v>0.0559505894780159</v>
       </c>
       <c r="E16" s="2">
-        <v>0.039570342749357224</v>
+        <v>0.034688640385866165</v>
       </c>
       <c r="F16" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H16" s="2">
-        <v>0.19173914194107056</v>
+        <v>-0.013426691293716431</v>
       </c>
       <c r="I16" s="2">
-        <v>0.35002052783966064</v>
+        <v>0.12532787024974823</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.2">
@@ -1109,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1121,7 +1124,7 @@
         <v>0.081302262842655182</v>
       </c>
       <c r="F23" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>17</v>
@@ -1138,7 +1141,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1150,7 +1153,7 @@
         <v>0.069241061806678772</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>17</v>
@@ -1167,7 +1170,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -1196,7 +1199,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1208,7 +1211,7 @@
         <v>0.067337781190872192</v>
       </c>
       <c r="F26" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>17</v>
@@ -1225,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1254,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
@@ -1266,7 +1269,7 @@
         <v>0.060195032507181168</v>
       </c>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>17</v>
@@ -1283,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
@@ -1312,7 +1315,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -1324,7 +1327,7 @@
         <v>0.035771388560533524</v>
       </c>
       <c r="F30" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>17</v>
@@ -1341,7 +1344,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -1353,7 +1356,7 @@
         <v>0.022104503586888313</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>17</v>
@@ -1370,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -1399,7 +1402,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1411,7 +1414,7 @@
         <v>0.031987257301807404</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>17</v>
@@ -1428,7 +1431,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1457,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
@@ -1469,7 +1472,7 @@
         <v>0.032154947519302368</v>
       </c>
       <c r="F35" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G35" t="s">
         <v>17</v>
@@ -1486,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>

</xml_diff>